<commit_message>
Adicionado Report em todos Cenários
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/HUB_BDD/DadosTeste/DadosTesteBDD.xlsx
+++ b/src/main/java/br/com/rsinet/HUB_BDD/DadosTeste/DadosTesteBDD.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{473C8DF7-06AB-43BA-BDA0-9D32F83155B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BC06A570-FC3A-4C27-BE0D-B250DEAAC02A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21030" windowHeight="11820" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20790" windowHeight="11820" xr2:uid="{B9FBF826-B1A8-476B-B191-287F00249889}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
     <t>Mesa</t>
   </si>
   <si>
-    <t>usertest210</t>
+    <t>testuser132</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>